<commit_message>
Change structure of robot to work with robocorp platform.
</commit_message>
<xml_diff>
--- a/Output/search_result.xlsx
+++ b/Output/search_result.xlsx
@@ -472,7 +472,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live news: Deadly combat rages as Rafah ...</t>
+          <t>Breaking News, World News and Video from Al Jazeera</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dollars of US aid and weaponry. “The other assistance that we've been providing for Israel's defence continues and will continue because</t>
+          <t>News, analysis from the Middle East &amp; worldwide, multimedia &amp; interactives, opinions, documentaries, podcasts, long reads and broadcast</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -498,7 +498,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Economy | Today's latest from Al Jazeera</t>
+          <t>Israel's war on Gaza live news: Attacks on besieged enclave kill 62 ...</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Russian court seizes two European banks' assets amid Western sanctions. Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas</t>
+          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -524,15 +524,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Breaking News, World News and Video from Al Jazeera</t>
+          <t>Economy | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45434</v>
+        <v>45433</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>News, analysis from the Middle East &amp; worldwide, multimedia &amp; interactives, opinions, documentaries, podcasts, long reads and broadcast</t>
+          <t>Russian court seizes two European banks' assets amid Western sanctions. Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -550,7 +550,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gaza war: What does victory look like for the US and Israel? | Israel ...</t>
+          <t>Israel's war on Gaza live news: Deadly combat rages as Rafah ...</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -558,7 +558,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Israel has said it is seeking an “absolute victory” over Hamas, as it continues to receive billions of dollars in unconditional military aid</t>
+          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -576,15 +576,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live news: Attacks on besieged enclave kill 62 ...</t>
+          <t>Gaza war: What does victory look like for the US and Israel? | Israel ...</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45434</v>
+        <v>45433</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
+          <t>Israel has said it is seeking an “absolute victory” over Hamas, as it continues to receive billions of dollars in unconditional military aid</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45432</v>
+        <v>45431</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
workitem test bug fix 3
</commit_message>
<xml_diff>
--- a/Output/search_result.xlsx
+++ b/Output/search_result.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Breaking News, World News and Video from Al Jazeera</t>
+          <t>Nvidia's profits soar as AI boom shows no sign of slowing down ...</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>News, analysis from the Middle East &amp; worldwide, multimedia &amp; interactives, opinions, documentaries, podcasts, long reads and broadcast</t>
+          <t>“Companies and countries are partnering with Nvidia to shift the trillion-dollar traditional data centres to accelerated computing and build</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -498,7 +498,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live news: Attacks on besieged enclave kill 62 ...</t>
+          <t>Breaking News, World News and Video from Al Jazeera</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
+          <t>News, analysis from the Middle East &amp; worldwide, multimedia &amp; interactives, opinions, documentaries, podcasts, long reads and broadcast</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -524,15 +524,15 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Economy | Today's latest from Al Jazeera</t>
+          <t>Israel's war on Gaza live news: Attacks on besieged enclave kill 62 ...</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45433</v>
+        <v>45434</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Russian court seizes two European banks' assets amid Western sanctions. Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas</t>
+          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -550,15 +550,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live news: Deadly combat rages as Rafah ...</t>
+          <t>Economy | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45434</v>
+        <v>45433</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
+          <t>Russian court seizes two European banks' assets amid Western sanctions. Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -576,15 +576,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Gaza war: What does victory look like for the US and Israel? | Israel ...</t>
+          <t>Israel's war on Gaza live news: Deadly combat rages as Rafah ...</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45433</v>
+        <v>45434</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Israel has said it is seeking an “absolute victory” over Hamas, as it continues to receive billions of dollars in unconditional military aid</t>
+          <t>Israel, a major recipient of US military assistance for decades, is still due to receive billions of dollars of US aid and weaponry. “The</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -602,15 +602,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Israel's war on Gaza live: UNRWA suspends food distribution in Rafah</t>
+          <t>Gaza war: What does victory look like for the US and Israel? | Israel ...</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45432</v>
+        <v>45433</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>dollars in US military assistance that remains in the pipeline for Prime Minister Benjamin Netanyahu's government. But Biden has also faced</t>
+          <t>Israel has said it is seeking an “absolute victory” over Hamas, as it continues to receive billions of dollars in unconditional military aid</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>'We love Taiwan': Domestic workers hope for more from new ...</t>
+          <t>Israel's war on Gaza live: UNRWA suspends food distribution in Rafah</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>While Taiwan's monthly minimum salary was increased to 27,470 New Taiwan dollars ($853) this year, migrant domestic workers, who also have to</t>
+          <t>dollars in US military assistance that remains in the pipeline for Prime Minister Benjamin Netanyahu's government. But Biden has also faced</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -648,21 +648,21 @@
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Who died alongside Iran's President Raisi in the helicopter crash ...</t>
+          <t>'We love Taiwan': Domestic workers hope for more from new ...</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45431</v>
+        <v>45432</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The AQR is a colossal bonyad, or charitable trust, that has billions of dollars in assets and is the custodian of the shrine of Imam Reza</t>
+          <t>While Taiwan's monthly minimum salary was increased to 27,470 New Taiwan dollars ($853) this year, migrant domestic workers, who also have to</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -674,13 +674,13 @@
         <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Iran helicopter crash updates: President Raisi, FM Amirabdollahian ...</t>
+          <t>Who died alongside Iran's President Raisi in the helicopter crash ...</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
@@ -688,7 +688,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>dollars, according to a Reuters investigation. Under Mokhber's watch, Setad developed Iran's coronavirus vaccine, Coviran Barekat, at the</t>
+          <t>The AQR is a colossal bonyad, or charitable trust, that has billions of dollars in assets and is the custodian of the shrine of Imam Reza</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -706,7 +706,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Who is Mohammad Mokhber, Iran's interim president? | Politics ...</t>
+          <t>Iran helicopter crash updates: President Raisi, FM Amirabdollahian ...</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
@@ -714,7 +714,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Mokhber led the Iranian supreme leader's multibillion-dollar charitable conglomerate for 14 years.</t>
+          <t>dollars, according to a Reuters investigation. Under Mokhber's watch, Setad developed Iran's coronavirus vaccine, Coviran Barekat, at the</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -732,7 +732,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ebrahim Raisi, Iran's president, dies in helicopter crash aged 63 ...</t>
+          <t>Who is Mohammad Mokhber, Iran's interim president? | Politics ...</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -740,7 +740,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The colossal bonyad, or charitable trust, has billions of dollars in assets and is the custodian of the shrine of Imam Reza, the eighth Shia</t>
+          <t>Mokhber led the Iranian supreme leader's multibillion-dollar charitable conglomerate for 14 years.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Panic in Bishkek: Why were Pakistani students attacked in ...</t>
+          <t>Ebrahim Raisi, Iran's president, dies in helicopter crash aged 63 ...</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -766,7 +766,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The Pakistani rupee, which stood at 160 against the US dollar in December 2020, has since slipped by more than 70 percent to 278 rupees a dollar</t>
+          <t>The colossal bonyad, or charitable trust, has billions of dollars in assets and is the custodian of the shrine of Imam Reza, the eighth Shia</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -784,15 +784,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Russian court seizes two European banks' assets amid Western ...</t>
+          <t>Panic in Bishkek: Why were Pakistani students attacked in ...</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45430</v>
+        <v>45431</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas project halted by sanctions.</t>
+          <t>The Pakistani rupee, which stood at 160 against the US dollar in December 2020, has since slipped by more than 70 percent to 278 rupees a dollar</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -810,15 +810,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lebanon's economic crisis endures, as does the EU's 'fear' of ...</t>
+          <t>Russian court seizes two European banks' assets amid Western ...</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45429</v>
+        <v>45430</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Billions of dollars go to the Syrian government, leaving it at the centre of the amphetamine's trade. Published On 10 Mar 202410 Mar 2024.</t>
+          <t>Freezing hundreds of billions of dollars in lenders' assets was part of dispute over gas project halted by sanctions.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -836,15 +836,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>What is Trident, the US floating pier off Gaza? Will it work? | Israel ...</t>
+          <t>Lebanon's economic crisis endures, as does the EU's 'fear' of ...</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45428</v>
+        <v>45429</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Washington has provided billions of dollars in aid as well as weapons that Israel has used in Gaza since October 7. Source: Al Jazeera</t>
+          <t>Billions of dollars go to the Syrian government, leaving it at the centre of the amphetamine's trade. Published On 10 Mar 202410 Mar 2024.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -862,7 +862,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Western volunteers join the battle against Myanmar's military regime ...</t>
+          <t>What is Trident, the US floating pier off Gaza? Will it work? | Israel ...</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
@@ -870,7 +870,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>dollar arsenal supplied by Russia and China. Ethnic armies, public donations and weapon seizures partly as a result of last year's Operation</t>
+          <t>Washington has provided billions of dollars in aid as well as weapons that Israel has used in Gaza since October 7. Source: Al Jazeera</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Republicans in US House pass bill pushing Biden to send weapons ...</t>
+          <t>Western volunteers join the battle against Myanmar's military regime ...</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Israel, a major recipient of US military assistance for decades, is still due to get billions of dollars of US weaponry, despite the delay</t>
+          <t>dollar arsenal supplied by Russia and China. Ethnic armies, public donations and weapon seizures partly as a result of last year's Operation</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -914,15 +914,15 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>US announces $2bn in new aid for Ukraine as Russian forces ...</t>
+          <t>Republicans in US House pass bill pushing Biden to send weapons ...</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45426</v>
+        <v>45428</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Antony Blinken says US rushing military support as Ukraine struggles to hold off renewed Russian offensive.</t>
+          <t>Israel, a major recipient of US military assistance for decades, is still due to get billions of dollars of US weaponry, despite the delay</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -931,16 +931,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Anxious Zimbabwean migrants, smugglers watch South Africa's ...</t>
+          <t>US announces $2bn in new aid for Ukraine as Russian forces ...</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
@@ -948,7 +948,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>The border province even favours using the South African rand, which people prefer to the local currency or the US dollar, which is popular</t>
+          <t>Antony Blinken says US rushing military support as Ukraine struggles to hold off renewed Russian offensive.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -957,16 +957,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Biden administration plans to send $1bn in military aid to Israel ...</t>
+          <t>Anxious Zimbabwean migrants, smugglers watch South Africa's ...</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
@@ -974,7 +974,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Request for tank ammunition, tactical vehicles for Israel despite Biden's earlier pause on bombs over Rafah assault.</t>
+          <t>The border province even favours using the South African rand, which people prefer to the local currency or the US dollar, which is popular</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -983,24 +983,24 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Russia's defence rejig: 'Unfortunately for Ukraine, a very effective ...</t>
+          <t>Biden administration plans to send $1bn in military aid to Israel ...</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>dollars on new weaponry and payments to servicemen and their families. “Putin needs an 'arsenal of autocracy' that can outperform Ukraine</t>
+          <t>Request for tank ammunition, tactical vehicles for Israel despite Biden's earlier pause on bombs over Rafah assault.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1009,16 +1009,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lawrence Wong set to take centre stage as Singapore's new prime ...</t>
+          <t>Russia's defence rejig: 'Unfortunately for Ukraine, a very effective ...</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>dollars ($1.6m) a year including bonuses. “Wong's biggest challenge in the short term will be to articulate an easy-to-understand, inclusive</t>
+          <t>dollars on new weaponry and payments to servicemen and their families. “Putin needs an 'arsenal of autocracy' that can outperform Ukraine</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1038,13 +1038,13 @@
         <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Not even the US government knows the US government line on ...</t>
+          <t>Lawrence Wong set to take centre stage as Singapore's new prime ...</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Of course, this money was authorised on top of the billions of dollars that the US already sends the country on an annual basis. When on May</t>
+          <t>dollars ($1.6m) a year including bonuses. “Wong's biggest challenge in the short term will be to articulate an easy-to-understand, inclusive</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1064,13 +1064,13 @@
         <v>1</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Boeing's jets turn 70: A timeline of highs, lows and turbulence ...</t>
+          <t>Not even the US government knows the US government line on ...</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>That same model rocket would be used for the Apollo 11 mission in 1969, landing astronauts on the moon. Boeing, the billion-dollar company.</t>
+          <t>Of course, this money was authorised on top of the billions of dollars that the US already sends the country on an annual basis. When on May</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1096,15 +1096,15 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>One of the biggest hurdles for athletes on the Olympic path: Money ...</t>
+          <t>Boeing's jets turn 70: A timeline of highs, lows and turbulence ...</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45424</v>
+        <v>45425</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>She declined to share the dollar figure for those costs as well. Lozano told Al Jazeera that she's using the funds from her GoFundMe</t>
+          <t>That same model rocket would be used for the Apollo 11 mission in 1969, landing astronauts on the moon. Boeing, the billion-dollar company.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1122,7 +1122,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Energy summit seeks to curb cooking habits that kill millions every ...</t>
+          <t>One of the biggest hurdles for athletes on the Olympic path: Money ...</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>dollars to fund expanded access to clean cooking methods.   “Dollar for dollar, it's hard to imagine a single intervention that</t>
+          <t>She declined to share the dollar figure for those costs as well. Lozano told Al Jazeera that she's using the funds from her GoFundMe</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -1148,7 +1148,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Top US Senator Bob Menendez's corruption trial begins | Courts ...</t>
+          <t>Energy summit seeks to curb cooking habits that kill millions every ...</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Prosecutors also said Menendez tried to help his other co-defendant, prominent New Jersey developer Fred Daibes, obtain millions of dollars</t>
+          <t>dollars to fund expanded access to clean cooking methods.   “Dollar for dollar, it's hard to imagine a single intervention that</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1226,15 +1226,15 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>'Climbing is for ladies too': Transforming Malawi into a climbers ...</t>
+          <t>What did Biden say about US arms transfers to Israel and what does ...</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45423</v>
+        <v>45420</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>In the last decade, climbing has gone from a niche sport to a worldwide sensation and multibillion-dollar industry. The sport made its debut</t>
+          <t>The US sends Israel $3.8bn in military aid annually, and Congress recently approved billions of dollars in additional support for the country.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1246,13 +1246,13 @@
         <v>1</v>
       </c>
       <c r="F31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>What did Biden say about US arms transfers to Israel and what does ...</t>
+          <t>After decades of decline, Air India is betting billions on a comeback ...</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>The US sends Israel $3.8bn in military aid annually, and Congress recently approved billions of dollars in additional support for the country.</t>
+          <t>In recent decades, India's national airline came to be seen as a cautionary tale of decline as it racked up billions of dollars in losses and</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1272,21 +1272,21 @@
         <v>1</v>
       </c>
       <c r="F32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>After decades of decline, Air India is betting billions on a comeback ...</t>
+          <t>Should India take from the rich, give the poor? A new election ...</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45420</v>
+        <v>45419</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>In recent decades, India's national airline came to be seen as a cautionary tale of decline as it racked up billions of dollars in losses and</t>
+          <t>Inequality was worsened over the past decade of Modi's rule. India has 271 dollar billionaires, third behind only China and the US — and world's</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1304,7 +1304,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Should India take from the rich, give the poor? A new election ...</t>
+          <t>Pentagon chief confirms US pause on weapons shipment to Israel ...</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Inequality was worsened over the past decade of Modi's rule. India has 271 dollar billionaires, third behind only China and the US — and world's</t>
+          <t>Over the years, the United States has provided tens of billions of dollars in military aid to Israel.” 'Iron-clad' support. The Biden</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1330,15 +1330,15 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Pentagon chief confirms US pause on weapons shipment to Israel ...</t>
+          <t>Zimbabwe's illegal forex dealers use WhatsApp to find clients, evade ...</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45419</v>
+        <v>45418</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Over the years, the United States has provided tens of billions of dollars in military aid to Israel.” 'Iron-clad' support. The Biden</t>
+          <t>dollar is the preferred medium of exchange. Everyone from state utilities to street vendors accepts payment in US dollars. Because of the</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1356,7 +1356,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Zimbabwe's illegal forex dealers use WhatsApp to find clients, evade ...</t>
+          <t>Boeing postpones launch of Starliner space capsule after technical ...</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>dollar is the preferred medium of exchange. Everyone from state utilities to street vendors accepts payment in US dollars. Because of the</t>
+          <t>NASA in 2014 awarded multibillion-dollar contracts to Boeing and SpaceX to develop space capsules for the space agency to ferry astronauts and</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -1382,15 +1382,15 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Boeing postpones launch of Starliner space capsule after technical ...</t>
+          <t>Australia's Qantas to pay $79m over 'ghost flights' furore | Aviation ...</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45418</v>
+        <v>45417</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NASA in 2014 awarded multibillion-dollar contracts to Boeing and SpaceX to develop space capsules for the space agency to ferry astronauts and</t>
+          <t>Australia's flagship airline Qantas has agreed to pay $120 million Australian dollars ($79m) to settle a lawsuit over the sale of tickets</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1402,32 +1402,6 @@
         <v>1</v>
       </c>
       <c r="F37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Australia's Qantas to pay $79m over 'ghost flights' furore | Aviation ...</t>
-        </is>
-      </c>
-      <c r="B38" s="2" t="n">
-        <v>45417</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Australia's flagship airline Qantas has agreed to pay $120 million Australian dollars ($79m) to settle a lawsuit over the sale of tickets</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>./Output/Images/36.jpg</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>